<commit_message>
Began readying app for API implementation and filled in spinner with list of genres from the API
</commit_message>
<xml_diff>
--- a/P4TestPlan.xlsx
+++ b/P4TestPlan.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/AndroidStudioProjects/CIS436P4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C2F093B-DE73-414A-B7DE-9D6C7A6B5580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101F67B8-65B0-D24F-866D-4F81CF985C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apr 24 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Apr 25 2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
   <si>
     <t>#</t>
   </si>
@@ -588,7 +590,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -709,6 +711,216 @@
       </c>
       <c r="I5" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B352A856-4A2F-CF4B-8839-FA6BF2557B90}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>44676</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">

</xml_diff>